<commit_message>
fix confusion between integer and number in schema_from_excel
</commit_message>
<xml_diff>
--- a/libs/client/cornflow_client/tests/data/xl_with_fk.xlsx
+++ b/libs/client/cornflow_client/tests/data/xl_with_fk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugo_larzabal\Documents\proyectos\cornflow\cornflow\libs\client\cornflow_client\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugo_larzabal\Documents\proyectos\cornflow\cornflow\libs\client\cornflow_client\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9434C719-DD88-4508-939A-266C3C90F4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1950348-FD1A-41E9-B370-A09B241674F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>32</v>
+        <v>32.1</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827E704E-1BC6-4E68-BA5A-8CFCB00C8E75}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +522,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,5 +592,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>